<commit_message>
Add 2 test cases for ebay electronics page.
</commit_message>
<xml_diff>
--- a/com.ebay/src/test/resources/TestData.xlsx
+++ b/com.ebay/src/test/resources/TestData.xlsx
@@ -1,32 +1,33 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24326"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10912"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hafiz\IDEA Project\Team1BootCamp\base\src\main\resources\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mdaziz/IdeaProjects/Team1BootCamp/com.ebay/src/test/resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4722EE68-90EB-42C0-AF92-D8B589C2F532}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0D92659A-0A4D-B547-B6B2-0147B2B05F62}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{BF43A26A-CFA6-4A10-8339-8D5564FBA255}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="19420" windowHeight="10420" activeTab="2" xr2:uid="{BF43A26A-CFA6-4A10-8339-8D5564FBA255}"/>
   </bookViews>
   <sheets>
     <sheet name="Expedia" sheetId="1" r:id="rId1"/>
-    <sheet name="Ebay" sheetId="2" r:id="rId2"/>
-    <sheet name="CBSSports" sheetId="3" r:id="rId3"/>
-    <sheet name="ATT" sheetId="4" r:id="rId4"/>
-    <sheet name="BankOfAmerica" sheetId="5" r:id="rId5"/>
-    <sheet name="BMWUSA" sheetId="6" r:id="rId6"/>
-    <sheet name="Trulia" sheetId="7" r:id="rId7"/>
-    <sheet name="AirBNB" sheetId="8" r:id="rId8"/>
-    <sheet name="OverStock" sheetId="9" r:id="rId9"/>
-    <sheet name="ESPN" sheetId="10" r:id="rId10"/>
-    <sheet name="Verizon" sheetId="11" r:id="rId11"/>
-    <sheet name="Chase" sheetId="12" r:id="rId12"/>
-    <sheet name="Mercedes-Benz" sheetId="13" r:id="rId13"/>
-    <sheet name="Redfin" sheetId="14" r:id="rId14"/>
+    <sheet name="Ebay" sheetId="15" r:id="rId2"/>
+    <sheet name="Ebay_Electronics" sheetId="2" r:id="rId3"/>
+    <sheet name="CBSSports" sheetId="3" r:id="rId4"/>
+    <sheet name="ATT" sheetId="4" r:id="rId5"/>
+    <sheet name="BankOfAmerica" sheetId="5" r:id="rId6"/>
+    <sheet name="BMWUSA" sheetId="6" r:id="rId7"/>
+    <sheet name="Trulia" sheetId="7" r:id="rId8"/>
+    <sheet name="AirBNB" sheetId="8" r:id="rId9"/>
+    <sheet name="OverStock" sheetId="9" r:id="rId10"/>
+    <sheet name="ESPN" sheetId="10" r:id="rId11"/>
+    <sheet name="Verizon" sheetId="11" r:id="rId12"/>
+    <sheet name="Chase" sheetId="12" r:id="rId13"/>
+    <sheet name="Mercedes-Benz" sheetId="13" r:id="rId14"/>
+    <sheet name="Redfin" sheetId="14" r:id="rId15"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -47,9 +48,57 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1" uniqueCount="1">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="17">
   <si>
     <t>A</t>
+  </si>
+  <si>
+    <t>ExpectedData</t>
+  </si>
+  <si>
+    <t>Electronics</t>
+  </si>
+  <si>
+    <t>Camera&amp;PhotoDropDown</t>
+  </si>
+  <si>
+    <t>Camera &amp; Photo Accessories</t>
+  </si>
+  <si>
+    <t>See all Cameras &amp; Photo</t>
+  </si>
+  <si>
+    <t>Camera Drones</t>
+  </si>
+  <si>
+    <t>DSLR Cameras</t>
+  </si>
+  <si>
+    <t>Mirrorless Digital Cameras</t>
+  </si>
+  <si>
+    <t>Point &amp; Shoot Digital Cameras</t>
+  </si>
+  <si>
+    <t>Film Cameras</t>
+  </si>
+  <si>
+    <t>Vintage Cameras</t>
+  </si>
+  <si>
+    <t>Action Camcorders</t>
+  </si>
+  <si>
+    <t>Camera Lenses</t>
+  </si>
+  <si>
+    <t>Telescopes</t>
+  </si>
+  <si>
+    <t>Cameras &amp; Photo</t>
+  </si>
+  <si>
+    <t>as</t>
   </si>
 </sst>
 </file>
@@ -403,15 +452,27 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2F16D271-5906-41EE-853E-85EA245B6942}">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C3A9241A-80CA-47A8-B8A7-CE843E51095C}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B2C6DB0C-125D-41E6-B672-3FA74959CDA8}">
   <dimension ref="A1"/>
   <sheetViews>
@@ -419,13 +480,13 @@
       <selection activeCell="K20" sqref="K20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9C4F54D1-3917-41AA-9115-54DFB60054C4}">
   <dimension ref="A1"/>
   <sheetViews>
@@ -433,13 +494,13 @@
       <selection activeCell="K20" sqref="K20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{71A4ED8F-84C7-4351-B184-022F160E827E}">
   <dimension ref="A1"/>
   <sheetViews>
@@ -447,13 +508,13 @@
       <selection activeCell="K21" sqref="K21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2BD1F144-5BE0-43B5-8C2F-943F03339C79}">
   <dimension ref="A1"/>
   <sheetViews>
@@ -461,13 +522,13 @@
       <selection activeCell="K19" sqref="K19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8C25186B-8AE5-4703-8BDB-6D9F1A2F53C3}">
   <dimension ref="A1"/>
   <sheetViews>
@@ -475,27 +536,153 @@
       <selection activeCell="K20" sqref="K20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C2BE8495-8323-FB4B-AE03-DE31202A238A}">
+  <dimension ref="A1:A2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:A2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>2</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9751B09C-FE73-4F13-A91B-81E55B55AAEA}">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D20" sqref="D20"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+  <dimension ref="A1:B12"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="24.6640625" customWidth="1"/>
+    <col min="2" max="2" width="22.6640625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B3" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>7</v>
+      </c>
+      <c r="B4" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>8</v>
+      </c>
+      <c r="B5" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>9</v>
+      </c>
+      <c r="B6" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>10</v>
+      </c>
+      <c r="B7" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>11</v>
+      </c>
+      <c r="B8" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>12</v>
+      </c>
+      <c r="B9" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>13</v>
+      </c>
+      <c r="B10" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>4</v>
+      </c>
+      <c r="B11" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>14</v>
+      </c>
+      <c r="B12" t="s">
+        <v>16</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{57A517B4-AB0A-4E50-8324-F3955FA294DA}">
   <dimension ref="A1"/>
   <sheetViews>
@@ -503,13 +690,13 @@
       <selection activeCell="E19" sqref="E19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0464987E-CA86-496F-AFAF-2580C40BA720}">
   <dimension ref="A1"/>
   <sheetViews>
@@ -517,13 +704,13 @@
       <selection activeCell="K18" sqref="K18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4DB124C4-9CEE-457F-95C0-47C63DA908AF}">
   <dimension ref="A1"/>
   <sheetViews>
@@ -531,9 +718,9 @@
       <selection activeCell="H20" sqref="H20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -543,7 +730,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5674FF68-7C81-4A9C-99FE-C7E070DBCFFA}">
   <dimension ref="A1"/>
   <sheetViews>
@@ -551,43 +738,31 @@
       <selection activeCell="H20" sqref="H20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AC436034-E141-4F6F-A259-658744C38455}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9F06E338-1C0F-45E0-B136-3FC6897D7CEC}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C3A9241A-80CA-47A8-B8A7-CE843E51095C}">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>